<commit_message>
Editing of data and mapper.json
</commit_message>
<xml_diff>
--- a/Data/2012/Volby 2012.xlsx
+++ b/Data/2012/Volby 2012.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eef0741620b644d4/Princípy datovej vedy/PROJEKT/Data/2012/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/eef0741620b644d4/Princípy datovej vedy/Projekt Git/PDV-Slovak-election-prediction/data/2012/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{3F101784-BFC0-4445-90E0-254B01171C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CBED175-AD53-438D-8CDF-34978600A3E5}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{3F101784-BFC0-4445-90E0-254B01171C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06ED0000-85EF-4C17-BC4A-8F1DD69BDA5D}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="4425" windowWidth="28800" windowHeight="15345" xr2:uid="{4CE25576-5E19-4F26-8F8C-FEF7BE50A434}"/>
+    <workbookView xWindow="38295" yWindow="0" windowWidth="7095" windowHeight="20985" xr2:uid="{4CE25576-5E19-4F26-8F8C-FEF7BE50A434}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -272,7 +272,7 @@
     <t>3 963</t>
   </si>
   <si>
-    <t>Polotický subjekt</t>
+    <t>Politický subjekt</t>
   </si>
 </sst>
 </file>
@@ -738,7 +738,7 @@
   <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>